<commit_message>
update package version rule
</commit_message>
<xml_diff>
--- a/doc/dev/package_version/version summary.xlsx
+++ b/doc/dev/package_version/version summary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\linshi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\azure-sdk-for-python\doc\dev\package_version\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C48BE5B6-C151-4B5D-82E6-DACE0F1688FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7257EA47-BE7E-4F88-BD9D-5F1ACCE74675}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{836FD595-2EBE-49F7-8D06-280877867AD6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{836FD595-2EBE-49F7-8D06-280877867AD6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,13 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="21">
-  <si>
-    <t>current version</t>
-  </si>
-  <si>
-    <t>tag type</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="22">
   <si>
     <t>changelog</t>
   </si>
@@ -98,6 +92,16 @@
   </si>
   <si>
     <t>2.0.0b1</t>
+  </si>
+  <si>
+    <t>last version</t>
+  </si>
+  <si>
+    <t>no stable
+ version</t>
+  </si>
+  <si>
+    <t>1.0.0</t>
   </si>
 </sst>
 </file>
@@ -168,20 +172,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -499,200 +509,200 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.21875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.44140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1" t="s">
+      <c r="E2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="6"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="7"/>
+      <c r="B6" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="3" t="s">
+      <c r="B7" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="1"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="4" t="s">
+      <c r="C7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="D7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="5" t="s">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="D8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="5" t="s">
+      <c r="D9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="6" t="s">
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="7"/>
+      <c r="B10" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4" t="s">
+      <c r="C10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="5" t="s">
         <v>8</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="4"/>
-      <c r="B10" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="A3:A6"/>
+    <mergeCell ref="B7:B9"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="A3:A8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="A7:A10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update package version rule (#29986)
* update package version rule

* update
</commit_message>
<xml_diff>
--- a/doc/dev/package_version/version summary.xlsx
+++ b/doc/dev/package_version/version summary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\linshi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\azure-sdk-for-python\doc\dev\package_version\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C48BE5B6-C151-4B5D-82E6-DACE0F1688FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7257EA47-BE7E-4F88-BD9D-5F1ACCE74675}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{836FD595-2EBE-49F7-8D06-280877867AD6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{836FD595-2EBE-49F7-8D06-280877867AD6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,13 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="21">
-  <si>
-    <t>current version</t>
-  </si>
-  <si>
-    <t>tag type</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="22">
   <si>
     <t>changelog</t>
   </si>
@@ -98,6 +92,16 @@
   </si>
   <si>
     <t>2.0.0b1</t>
+  </si>
+  <si>
+    <t>last version</t>
+  </si>
+  <si>
+    <t>no stable
+ version</t>
+  </si>
+  <si>
+    <t>1.0.0</t>
   </si>
 </sst>
 </file>
@@ -168,20 +172,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -499,200 +509,200 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.21875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.44140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1" t="s">
+      <c r="E2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="6"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="7"/>
+      <c r="B6" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="3" t="s">
+      <c r="B7" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="1"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="4" t="s">
+      <c r="C7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="D7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="5" t="s">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="D8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="5" t="s">
+      <c r="D9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="6" t="s">
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="7"/>
+      <c r="B10" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4" t="s">
+      <c r="C10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="5" t="s">
         <v>8</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="4"/>
-      <c r="B10" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="A3:A6"/>
+    <mergeCell ref="B7:B9"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="A3:A8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="A7:A10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>